<commit_message>
Revisi Gant Chart dan WBS
- Mengganti gant chart yang lama dan WBS yang lama dengan yang baru
- Menghapus file yang tidak penting
</commit_message>
<xml_diff>
--- a/GantChart.xlsx
+++ b/GantChart.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="50">
   <si>
     <t/>
   </si>
@@ -66,7 +66,7 @@
     <t>Membuat user stories</t>
   </si>
   <si>
-    <t>Buat task,Estimasi  dan Sprint backlog</t>
+    <t>Buat task,Estimasi, Software Model,  dan Sprint backlog</t>
   </si>
   <si>
     <t>Sprint 1</t>
@@ -75,19 +75,19 @@
     <t>20d</t>
   </si>
   <si>
-    <t>Membuat class diagram</t>
+    <t>Update Task</t>
   </si>
   <si>
     <t>4d</t>
   </si>
   <si>
-    <t>Develop Authentication</t>
+    <t>Develop fitur profile</t>
   </si>
   <si>
     <t>3d</t>
   </si>
   <si>
-    <t>Develop fitur Home</t>
+    <t>Develop fitur schedule</t>
   </si>
   <si>
     <t>9d</t>
@@ -96,7 +96,7 @@
     <t>10; 5</t>
   </si>
   <si>
-    <t>Develop profil</t>
+    <t>Develop fitur reminder</t>
   </si>
   <si>
     <t>Testing fitur sprint1</t>
@@ -111,16 +111,16 @@
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Update Task</t>
-  </si>
-  <si>
-    <t>Develop fitur  Food Calories</t>
+    <t>Sprint Review, Evaluation, &amp; Update Task</t>
+  </si>
+  <si>
+    <t>Develop fitur  food calories</t>
   </si>
   <si>
     <t>11d</t>
   </si>
   <si>
-    <t>Develop fitur food Recomendation</t>
+    <t>Develop fitur home</t>
   </si>
   <si>
     <t>Testing fitur Sprint 2</t>
@@ -135,13 +135,10 @@
     <t>24d</t>
   </si>
   <si>
-    <t>Sprint Review, Evaluation</t>
-  </si>
-  <si>
-    <t>Develop fitur Reminder</t>
-  </si>
-  <si>
-    <t>Develop fitur Week Evaluation, Share</t>
+    <t>Develop fitur week evaluation</t>
+  </si>
+  <si>
+    <t>Develop fitur food recommendation</t>
   </si>
   <si>
     <t>Testing fitur sprint 3</t>
@@ -162,7 +159,7 @@
     <t>Jenny Gruening</t>
   </si>
   <si>
-    <t>27/06/13 23:02</t>
+    <t>27/06/13 9:02</t>
   </si>
   <si>
     <t>You can add discussions, notes, or emails to discussions.</t>
@@ -858,7 +855,7 @@
     <row r="23" hidden="false" outlineLevel="1">
       <c r="A23" s="3"/>
       <c r="B23" t="s" s="29">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C23" t="n" s="31">
         <v>42500.0</v>
@@ -876,7 +873,7 @@
     <row r="24" hidden="false" outlineLevel="1">
       <c r="A24" s="3"/>
       <c r="B24" t="s" s="29">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" t="n" s="31">
         <v>42503.0</v>
@@ -894,7 +891,7 @@
     <row r="25" hidden="false" outlineLevel="1">
       <c r="A25" s="3"/>
       <c r="B25" t="s" s="29">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="n" s="31">
         <v>42503.0</v>
@@ -912,7 +909,7 @@
     <row r="26" hidden="false" outlineLevel="1">
       <c r="A26" s="3"/>
       <c r="B26" t="s" s="29">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="n" s="31">
         <v>42518.0</v>
@@ -930,7 +927,7 @@
     <row r="27" hidden="false" outlineLevel="1">
       <c r="A27" s="3"/>
       <c r="B27" t="s" s="29">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="n" s="31">
         <v>42521.0</v>
@@ -967,19 +964,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2">
@@ -987,13 +984,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
         <v>48</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3"/>

</xml_diff>